<commit_message>
Excel sheet for whitebox, blackbox & greybox testing
</commit_message>
<xml_diff>
--- a/Burndown Chart.xlsx
+++ b/Burndown Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SD6503_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057C835B-29A0-492E-9C0D-2405F04DEA58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF2C844-6682-4D40-8F84-E7C34AAD8CDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>BurnDownChart Sprint 1</a:t>
+              <a:t>BurnDownChart Sprint 4</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -230,25 +230,25 @@
                 <c:formatCode>d\-mmm</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44102</c:v>
+                  <c:v>44123</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44103</c:v>
+                  <c:v>44124</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44104</c:v>
+                  <c:v>44125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44105</c:v>
+                  <c:v>44126</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44106</c:v>
+                  <c:v>44127</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44107</c:v>
+                  <c:v>44128</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44108</c:v>
+                  <c:v>44129</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -260,22 +260,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.833333333333332</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.666666666666666</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.5</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.333333333333333</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.1666666666666665</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -335,25 +335,25 @@
                 <c:formatCode>d\-mmm</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44102</c:v>
+                  <c:v>44123</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44103</c:v>
+                  <c:v>44124</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44104</c:v>
+                  <c:v>44125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44105</c:v>
+                  <c:v>44126</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44106</c:v>
+                  <c:v>44127</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44107</c:v>
+                  <c:v>44128</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44108</c:v>
+                  <c:v>44129</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -368,22 +368,22 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1485,7 +1485,7 @@
   <dimension ref="A3:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1542,10 +1542,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>44102</v>
+        <v>44123</v>
       </c>
       <c r="B15">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <v>15</v>
@@ -1553,23 +1553,23 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>44103</v>
+        <v>44124</v>
       </c>
       <c r="B16">
-        <f xml:space="preserve"> (19/6) * 5</f>
-        <v>15.833333333333332</v>
+        <f xml:space="preserve"> (15/6) * 5</f>
+        <v>12.5</v>
       </c>
       <c r="C16">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>44104</v>
+        <v>44125</v>
       </c>
       <c r="B17">
-        <f xml:space="preserve"> (19/6) * 4</f>
-        <v>12.666666666666666</v>
+        <f xml:space="preserve"> (15/6) * 4</f>
+        <v>10</v>
       </c>
       <c r="C17">
         <v>11</v>
@@ -1577,49 +1577,49 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>44105</v>
+        <v>44126</v>
       </c>
       <c r="B18">
-        <f xml:space="preserve"> (19/6) * 3</f>
-        <v>9.5</v>
+        <f xml:space="preserve"> (15/6) * 3</f>
+        <v>7.5</v>
       </c>
       <c r="C18">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>44106</v>
+        <v>44127</v>
       </c>
       <c r="B19">
-        <f xml:space="preserve"> (19/6) * 2</f>
-        <v>6.333333333333333</v>
+        <f xml:space="preserve"> (15/6) * 2</f>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>44107</v>
+        <v>44128</v>
       </c>
       <c r="B20">
-        <f xml:space="preserve"> (19/6) * 1</f>
-        <v>3.1666666666666665</v>
+        <f xml:space="preserve"> (15/6) * 1</f>
+        <v>2.5</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>44108</v>
+        <v>44129</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>